<commit_message>
Updated Configuration.xlsx template file
</commit_message>
<xml_diff>
--- a/templates/Configuration.xlsx
+++ b/templates/Configuration.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/d287d90c9afa643e/Documentos/Softtek Work/all_track/SOLID_Code/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/d287d90c9afa643e/Documentos/Working/qa-report-generator/templates/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="207" documentId="8_{5B33C681-5304-4961-A816-5F9ABDB4C3CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3F667B0B-4737-4210-853B-FDED4806ED16}"/>
+  <xr:revisionPtr revIDLastSave="456" documentId="8_{5B33C681-5304-4961-A816-5F9ABDB4C3CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8B79DDD0-C6F1-4CEF-A9E5-8EBBFD4520A4}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{7794AE0A-77F5-4F9D-8122-2E0B65EAAC73}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{7794AE0A-77F5-4F9D-8122-2E0B65EAAC73}"/>
   </bookViews>
   <sheets>
     <sheet name="Sprints" sheetId="1" r:id="rId1"/>
@@ -93,7 +93,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="27">
   <si>
     <t>Sprint No</t>
   </si>
@@ -125,12 +125,6 @@
     <t>Specify the period to be reported</t>
   </si>
   <si>
-    <t>Month</t>
-  </si>
-  <si>
-    <t>Year</t>
-  </si>
-  <si>
     <t>Module/Feature</t>
   </si>
   <si>
@@ -143,9 +137,6 @@
     <t>Specify Report File Name</t>
   </si>
   <si>
-    <t>May</t>
-  </si>
-  <si>
     <t>1-0000030767-1</t>
   </si>
   <si>
@@ -180,6 +171,9 @@
   </si>
   <si>
     <t>bruce.banner</t>
+  </si>
+  <si>
+    <t>Last Id Number</t>
   </si>
 </sst>
 </file>
@@ -380,34 +374,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color theme="3" tint="0.249977111117893"/>
-      </right>
-      <top style="thin">
-        <color theme="3" tint="0.249977111117893"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color theme="3" tint="0.249977111117893"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color theme="3" tint="0.249977111117893"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
       <top style="thin">
@@ -442,11 +408,33 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color theme="3" tint="0.249977111117893"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color theme="3" tint="0.249977111117893"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color theme="3" tint="0.249977111117893"/>
+      </right>
+      <top style="thin">
+        <color theme="3" tint="0.249977111117893"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -481,7 +469,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -492,9 +480,6 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -508,42 +493,55 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="18" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="14" fontId="0" fillId="3" borderId="9" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="17">
+  <dxfs count="18">
     <dxf>
       <font>
-        <color rgb="FF9C0006"/>
+        <sz val="10"/>
       </font>
+      <numFmt numFmtId="2" formatCode="0.00"/>
       <fill>
         <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
         </patternFill>
       </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom/>
+      </border>
     </dxf>
     <dxf>
       <font>
@@ -557,7 +555,7 @@
         </patternFill>
       </fill>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
+      <border diagonalUp="0" diagonalDown="0" outline="0">
         <left style="thin">
           <color indexed="64"/>
         </left>
@@ -568,9 +566,27 @@
           <color indexed="64"/>
         </top>
         <bottom/>
-        <vertical/>
-        <horizontal/>
       </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
     </dxf>
     <dxf>
       <font>
@@ -801,17 +817,89 @@
 </styleSheet>
 </file>
 
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>57150</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>138111</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>304800</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>161924</xdr:rowOff>
+    </xdr:to>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:we="http://schemas.microsoft.com/office/webextensions/webextension/2010/11" Requires="we">
+        <xdr:graphicFrame macro="">
+          <xdr:nvGraphicFramePr>
+            <xdr:cNvPr id="3" name="Add-in 2">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D7C574F8-7014-AA15-7EE3-B21C427BA7EE}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvGraphicFramePr>
+              <a:graphicFrameLocks noGrp="1"/>
+            </xdr:cNvGraphicFramePr>
+          </xdr:nvGraphicFramePr>
+          <xdr:xfrm>
+            <a:off x="0" y="0"/>
+            <a:ext cx="0" cy="0"/>
+          </xdr:xfrm>
+          <a:graphic>
+            <a:graphicData uri="http://schemas.microsoft.com/office/webextensions/webextension/2010/11">
+              <we:webextensionref xmlns:we="http://schemas.microsoft.com/office/webextensions/webextension/2010/11" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+            </a:graphicData>
+          </a:graphic>
+        </xdr:graphicFrame>
+      </mc:Choice>
+      <mc:Fallback>
+        <xdr:pic>
+          <xdr:nvPicPr>
+            <xdr:cNvPr id="3" name="Add-in 2">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D7C574F8-7014-AA15-7EE3-B21C427BA7EE}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvPicPr/>
+          </xdr:nvPicPr>
+          <xdr:blipFill>
+            <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+            <a:stretch>
+              <a:fillRect/>
+            </a:stretch>
+          </xdr:blipFill>
+          <xdr:spPr>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+          </xdr:spPr>
+        </xdr:pic>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
 <personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{36937B47-E3C7-4E44-8EBC-C7BBA3744F04}" name="Sprints" displayName="Sprints" ref="A1:C7" totalsRowShown="0" headerRowDxfId="16" dataDxfId="15">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{36937B47-E3C7-4E44-8EBC-C7BBA3744F04}" name="Sprints" displayName="Sprints" ref="A1:C7" totalsRowShown="0" headerRowDxfId="17" dataDxfId="16">
   <autoFilter ref="A1:C7" xr:uid="{36937B47-E3C7-4E44-8EBC-C7BBA3744F04}"/>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{FCC1C8C2-3D7D-4BC4-893F-703247F23159}" name="Sprint No" dataDxfId="14"/>
-    <tableColumn id="2" xr3:uid="{9E6CF723-3B7A-4B97-888D-18B4C4E8CEA6}" name="Start Date" dataDxfId="13"/>
-    <tableColumn id="3" xr3:uid="{D241FA2E-C984-4980-8612-1D058EA33128}" name="End Date" dataDxfId="12">
+    <tableColumn id="1" xr3:uid="{FCC1C8C2-3D7D-4BC4-893F-703247F23159}" name="Sprint No" dataDxfId="15"/>
+    <tableColumn id="2" xr3:uid="{9E6CF723-3B7A-4B97-888D-18B4C4E8CEA6}" name="Start Date" dataDxfId="14"/>
+    <tableColumn id="3" xr3:uid="{D241FA2E-C984-4980-8612-1D058EA33128}" name="End Date" dataDxfId="13">
       <calculatedColumnFormula>Sprints[[#This Row],[Start Date]]+13</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -820,14 +908,15 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{36CEC4BE-9F59-4258-BAE7-3A3731050C3D}" name="TM" displayName="TM" ref="A1:E6" totalsRowShown="0" headerRowDxfId="11" dataDxfId="9" headerRowBorderDxfId="10" tableBorderDxfId="8" totalsRowBorderDxfId="7">
-  <autoFilter ref="A1:E6" xr:uid="{36CEC4BE-9F59-4258-BAE7-3A3731050C3D}"/>
-  <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{A23692DF-DE16-42F9-841D-0DF27E9100D2}" name="Project ID" dataDxfId="6"/>
-    <tableColumn id="2" xr3:uid="{C9F00292-5BFC-4C6A-9A97-5455BF047CA5}" name="Team Member" dataDxfId="5"/>
-    <tableColumn id="4" xr3:uid="{875444D6-04B5-4C66-AE64-C2D0E852B4F2}" name="Peer Reviewer" dataDxfId="4"/>
-    <tableColumn id="5" xr3:uid="{3435DD14-C5E3-49EE-8C4D-C868E72AFDD6}" name="Testing Type" dataDxfId="3"/>
-    <tableColumn id="3" xr3:uid="{D74B2154-8F05-428C-B793-B6466631BD14}" name="Module/Feature" dataDxfId="2"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{36CEC4BE-9F59-4258-BAE7-3A3731050C3D}" name="TM" displayName="TM" ref="A1:F6" totalsRowShown="0" headerRowDxfId="12" dataDxfId="10" headerRowBorderDxfId="11" tableBorderDxfId="9" totalsRowBorderDxfId="8">
+  <autoFilter ref="A1:F6" xr:uid="{36CEC4BE-9F59-4258-BAE7-3A3731050C3D}"/>
+  <tableColumns count="6">
+    <tableColumn id="1" xr3:uid="{A23692DF-DE16-42F9-841D-0DF27E9100D2}" name="Project ID" dataDxfId="7"/>
+    <tableColumn id="2" xr3:uid="{C9F00292-5BFC-4C6A-9A97-5455BF047CA5}" name="Team Member" dataDxfId="6"/>
+    <tableColumn id="4" xr3:uid="{875444D6-04B5-4C66-AE64-C2D0E852B4F2}" name="Peer Reviewer" dataDxfId="5"/>
+    <tableColumn id="5" xr3:uid="{3435DD14-C5E3-49EE-8C4D-C868E72AFDD6}" name="Testing Type" dataDxfId="4"/>
+    <tableColumn id="3" xr3:uid="{D74B2154-8F05-428C-B793-B6466631BD14}" name="Module/Feature" dataDxfId="1"/>
+    <tableColumn id="6" xr3:uid="{7E06EBC5-0B3D-4211-B09A-97E01DCBEE14}" name="Last Id Number" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium15" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1148,6 +1237,20 @@
 </a:theme>
 </file>
 
+<file path=xl/webextensions/webextension1.xml><?xml version="1.0" encoding="utf-8"?>
+<we:webextension xmlns:we="http://schemas.microsoft.com/office/webextensions/webextension/2010/11" id="{D7C574F8-7014-AA15-7EE3-B21C427BA7EE}">
+  <we:reference id="wa102957665" version="1.3.0.0" store="en-US" storeType="OMEX"/>
+  <we:alternateReferences>
+    <we:reference id="wa102957665" version="1.3.0.0" store="wa102957665" storeType="OMEX"/>
+  </we:alternateReferences>
+  <we:properties>
+    <we:property name="opt_month" value="&quot;2024-05-01&quot;"/>
+  </we:properties>
+  <we:bindings/>
+  <we:snapshot xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+</we:webextension>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2C413FB2-15FD-40C5-9896-7E0B02C3279F}">
   <dimension ref="A1:C7"/>
@@ -1163,13 +1266,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" s="20" t="s">
+      <c r="A1" s="19" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="20" t="s">
+      <c r="B1" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="20" t="s">
+      <c r="C1" s="19" t="s">
         <v>2</v>
       </c>
     </row>
@@ -1177,10 +1280,10 @@
       <c r="A2" s="8">
         <v>6.1</v>
       </c>
-      <c r="B2" s="17">
+      <c r="B2" s="16">
         <v>45379</v>
       </c>
-      <c r="C2" s="17">
+      <c r="C2" s="16">
         <f>Sprints[[#This Row],[Start Date]]+13</f>
         <v>45392</v>
       </c>
@@ -1189,10 +1292,10 @@
       <c r="A3" s="8">
         <v>6.2</v>
       </c>
-      <c r="B3" s="17">
+      <c r="B3" s="16">
         <v>45393</v>
       </c>
-      <c r="C3" s="17">
+      <c r="C3" s="16">
         <f>Sprints[[#This Row],[Start Date]]+13</f>
         <v>45406</v>
       </c>
@@ -1201,10 +1304,10 @@
       <c r="A4" s="8">
         <v>6.3</v>
       </c>
-      <c r="B4" s="17">
+      <c r="B4" s="16">
         <v>45407</v>
       </c>
-      <c r="C4" s="17">
+      <c r="C4" s="16">
         <f>Sprints[[#This Row],[Start Date]]+13</f>
         <v>45420</v>
       </c>
@@ -1213,10 +1316,10 @@
       <c r="A5" s="8">
         <v>6.4</v>
       </c>
-      <c r="B5" s="17">
+      <c r="B5" s="16">
         <v>45421</v>
       </c>
-      <c r="C5" s="17">
+      <c r="C5" s="16">
         <f>Sprints[[#This Row],[Start Date]]+13</f>
         <v>45434</v>
       </c>
@@ -1225,30 +1328,30 @@
       <c r="A6" s="8">
         <v>6.5</v>
       </c>
-      <c r="B6" s="18">
+      <c r="B6" s="17">
         <v>45435</v>
       </c>
-      <c r="C6" s="17">
+      <c r="C6" s="16">
         <f>Sprints[[#This Row],[Start Date]]+13</f>
         <v>45448</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" s="19">
+      <c r="A7" s="18">
         <v>6.6</v>
       </c>
-      <c r="B7" s="17">
+      <c r="B7" s="16">
         <v>45449</v>
       </c>
-      <c r="C7" s="17">
+      <c r="C7" s="16">
         <f>Sprints[[#This Row],[Start Date]]+13</f>
         <v>45462</v>
       </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="B1:B7">
-    <cfRule type="duplicateValues" dxfId="1" priority="1"/>
-    <cfRule type="duplicateValues" dxfId="0" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="3" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="2" priority="2"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
@@ -1261,8 +1364,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F751ADBD-BE5E-454F-B8E3-111BA825410E}">
   <dimension ref="A1:Z6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B29" sqref="B29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1272,6 +1375,7 @@
     <col min="3" max="3" width="18.5703125" customWidth="1"/>
     <col min="4" max="4" width="17" customWidth="1"/>
     <col min="5" max="5" width="18.42578125" customWidth="1"/>
+    <col min="6" max="6" width="21" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="27" customHeight="1" x14ac:dyDescent="0.25">
@@ -1288,25 +1392,31 @@
         <v>6</v>
       </c>
       <c r="E1" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="Z1" s="21"/>
+        <v>10</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="Z1" s="20"/>
     </row>
     <row r="2" spans="1:26" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
         <v>7</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="D2" s="6" t="s">
         <v>8</v>
       </c>
       <c r="E2" s="6" t="s">
-        <v>14</v>
+        <v>12</v>
+      </c>
+      <c r="F2" s="28">
+        <v>165</v>
       </c>
     </row>
     <row r="3" spans="1:26" ht="24" customHeight="1" x14ac:dyDescent="0.25">
@@ -1314,16 +1424,19 @@
         <v>7</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="D3" s="6" t="s">
         <v>8</v>
       </c>
       <c r="E3" s="6" t="s">
-        <v>14</v>
+        <v>12</v>
+      </c>
+      <c r="F3" s="28">
+        <v>165</v>
       </c>
     </row>
     <row r="4" spans="1:26" ht="24" customHeight="1" x14ac:dyDescent="0.25">
@@ -1331,50 +1444,59 @@
         <v>7</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="D4" s="6" t="s">
         <v>8</v>
       </c>
       <c r="E4" s="6" t="s">
-        <v>13</v>
+        <v>11</v>
+      </c>
+      <c r="F4" s="28">
+        <v>165</v>
       </c>
     </row>
     <row r="5" spans="1:26" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="D5" s="6" t="s">
         <v>8</v>
       </c>
       <c r="E5" s="6" t="s">
-        <v>18</v>
+        <v>15</v>
+      </c>
+      <c r="F5" s="28">
+        <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:26" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="D6" s="6" t="s">
         <v>8</v>
       </c>
       <c r="E6" s="6" t="s">
-        <v>20</v>
+        <v>17</v>
+      </c>
+      <c r="F6" s="28">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -1388,10 +1510,11 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B3843A5F-DCEB-4AD8-B35D-1B088BF336A0}">
-  <dimension ref="B2:E23"/>
+  <sheetPr codeName="Sheet1"/>
+  <dimension ref="B2:J25"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="D27" sqref="D27:D28"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="F35" sqref="F35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1401,103 +1524,112 @@
     <col min="3" max="3" width="19.28515625" customWidth="1"/>
     <col min="4" max="4" width="19.28515625" style="7" customWidth="1"/>
     <col min="5" max="5" width="1" customWidth="1"/>
+    <col min="7" max="7" width="16.85546875" customWidth="1"/>
+    <col min="10" max="10" width="13.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B2" s="14"/>
-      <c r="C2" s="22" t="s">
+      <c r="C2" s="24" t="s">
         <v>9</v>
       </c>
-      <c r="D2" s="23"/>
+      <c r="D2" s="25"/>
       <c r="E2" s="13"/>
     </row>
-    <row r="3" spans="2:5" ht="4.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:7" ht="4.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="14"/>
       <c r="C3" s="12"/>
       <c r="D3" s="11"/>
     </row>
-    <row r="4" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:7" x14ac:dyDescent="0.25">
       <c r="D4" s="10"/>
     </row>
-    <row r="5" spans="2:5" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:7" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B5" s="14"/>
       <c r="C5" s="9" t="s">
-        <v>10</v>
-      </c>
-      <c r="D5" s="16" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="6" spans="2:5" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+      <c r="D5" s="23">
+        <v>45440</v>
+      </c>
+      <c r="F5" s="21"/>
+      <c r="G5" s="21"/>
+    </row>
+    <row r="6" spans="2:7" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B6" s="14"/>
       <c r="C6" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="D6" s="16">
-        <v>2024</v>
-      </c>
-    </row>
-    <row r="7" spans="2:5" ht="4.5" customHeight="1" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+      <c r="D6" s="23">
+        <v>45441</v>
+      </c>
+    </row>
+    <row r="7" spans="2:7" ht="4.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B7" s="14"/>
       <c r="C7" s="14"/>
       <c r="D7" s="15"/>
     </row>
-    <row r="10" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B10" s="14"/>
-      <c r="C10" s="22" t="s">
-        <v>15</v>
-      </c>
-      <c r="D10" s="23"/>
-    </row>
-    <row r="11" spans="2:5" ht="4.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C10" s="24" t="s">
+        <v>13</v>
+      </c>
+      <c r="D10" s="25"/>
+    </row>
+    <row r="11" spans="2:7" ht="4.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B11" s="14"/>
       <c r="C11" s="14"/>
       <c r="D11" s="15"/>
     </row>
-    <row r="12" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="13" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C13" s="24" t="s">
-        <v>23</v>
-      </c>
-      <c r="D13" s="25"/>
-    </row>
-    <row r="15" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="13" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C13" s="26" t="s">
+        <v>20</v>
+      </c>
+      <c r="D13" s="27"/>
+    </row>
+    <row r="15" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B15" s="14"/>
-      <c r="C15" s="22" t="s">
-        <v>21</v>
-      </c>
-      <c r="D15" s="23"/>
-    </row>
-    <row r="16" spans="2:5" ht="4.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C15" s="24" t="s">
+        <v>18</v>
+      </c>
+      <c r="D15" s="25"/>
+    </row>
+    <row r="16" spans="2:7" ht="4.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B16" s="14"/>
       <c r="C16" s="14"/>
       <c r="D16" s="15"/>
     </row>
-    <row r="17" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="18" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C18" s="24" t="s">
+    <row r="17" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="18" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C18" s="26" t="s">
         <v>7</v>
       </c>
-      <c r="D18" s="25"/>
-    </row>
-    <row r="20" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="D18" s="27"/>
+    </row>
+    <row r="20" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B20" s="14"/>
-      <c r="C20" s="22" t="s">
-        <v>22</v>
-      </c>
-      <c r="D20" s="23"/>
-    </row>
-    <row r="21" spans="2:4" ht="4.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C20" s="24" t="s">
+        <v>19</v>
+      </c>
+      <c r="D20" s="25"/>
+      <c r="G20" s="21"/>
+    </row>
+    <row r="21" spans="2:10" ht="4.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B21" s="14"/>
       <c r="C21" s="14"/>
       <c r="D21" s="15"/>
     </row>
-    <row r="22" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="23" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C23" s="24">
-        <v>15</v>
-      </c>
-      <c r="D23" s="25"/>
+    <row r="22" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="23" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C23" s="26">
+        <f>_xlfn.XLOOKUP(C18,TM[Project ID],TM[Last Id Number])</f>
+        <v>165</v>
+      </c>
+      <c r="D23" s="27"/>
+    </row>
+    <row r="25" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="J25" s="22"/>
     </row>
   </sheetData>
   <mergeCells count="7">
@@ -1509,17 +1641,12 @@
     <mergeCell ref="C15:D15"/>
     <mergeCell ref="C18:D18"/>
   </mergeCells>
-  <dataValidations count="3">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D5" xr:uid="{7E71CE15-1241-4A21-9001-54F8A67CE430}">
-      <formula1>"January, February, March, April, May, June, July, August, September, October, November, December"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D6" xr:uid="{1A49E044-6C57-4AC9-A08A-91D17144C727}">
-      <formula1>"2024, 2025"</formula1>
-    </dataValidation>
+  <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Choose the wbs" sqref="C18:D18" xr:uid="{126A9041-2396-416D-A6EE-B0E67E84C713}">
       <formula1>INDIRECT("TM[Project ID]")</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>